<commit_message>
updating with new data
</commit_message>
<xml_diff>
--- a/py_outputs/geo_country.xlsx
+++ b/py_outputs/geo_country.xlsx
@@ -44,12 +44,12 @@
     <t xml:space="preserve">jpn</t>
   </si>
   <si>
+    <t xml:space="preserve">chn</t>
+  </si>
+  <si>
     <t xml:space="preserve">esp</t>
   </si>
   <si>
-    <t xml:space="preserve">chn</t>
-  </si>
-  <si>
     <t xml:space="preserve">can</t>
   </si>
   <si>
@@ -83,15 +83,15 @@
     <t xml:space="preserve">rus</t>
   </si>
   <si>
+    <t xml:space="preserve">twn</t>
+  </si>
+  <si>
     <t xml:space="preserve">pol</t>
   </si>
   <si>
     <t xml:space="preserve">fin</t>
   </si>
   <si>
-    <t xml:space="preserve">twn</t>
-  </si>
-  <si>
     <t xml:space="preserve">aut</t>
   </si>
   <si>
@@ -119,42 +119,42 @@
     <t xml:space="preserve">cze</t>
   </si>
   <si>
+    <t xml:space="preserve">irn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sgp</t>
+  </si>
+  <si>
     <t xml:space="preserve">irl</t>
   </si>
   <si>
-    <t xml:space="preserve">sgp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">irn</t>
-  </si>
-  <si>
     <t xml:space="preserve">chl</t>
   </si>
   <si>
     <t xml:space="preserve">arg</t>
   </si>
   <si>
+    <t xml:space="preserve">sau</t>
+  </si>
+  <si>
     <t xml:space="preserve">hun</t>
   </si>
   <si>
-    <t xml:space="preserve">sau</t>
-  </si>
-  <si>
     <t xml:space="preserve">nzl</t>
   </si>
   <si>
+    <t xml:space="preserve">egy</t>
+  </si>
+  <si>
     <t xml:space="preserve">tha</t>
   </si>
   <si>
+    <t xml:space="preserve">hkg</t>
+  </si>
+  <si>
     <t xml:space="preserve">rou</t>
   </si>
   <si>
-    <t xml:space="preserve">hkg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egy</t>
-  </si>
-  <si>
     <t xml:space="preserve">pak</t>
   </si>
   <si>
@@ -167,30 +167,30 @@
     <t xml:space="preserve">nga</t>
   </si>
   <si>
+    <t xml:space="preserve">idn</t>
+  </si>
+  <si>
     <t xml:space="preserve">hrv</t>
   </si>
   <si>
-    <t xml:space="preserve">idn</t>
+    <t xml:space="preserve">vnm</t>
   </si>
   <si>
     <t xml:space="preserve">srb</t>
   </si>
   <si>
-    <t xml:space="preserve">vnm</t>
-  </si>
-  <si>
     <t xml:space="preserve">svn</t>
   </si>
   <si>
+    <t xml:space="preserve">ken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per</t>
+  </si>
+  <si>
     <t xml:space="preserve">svk</t>
   </si>
   <si>
-    <t xml:space="preserve">ken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">per</t>
-  </si>
-  <si>
     <t xml:space="preserve">ukr</t>
   </si>
   <si>
@@ -200,27 +200,27 @@
     <t xml:space="preserve">bgr</t>
   </si>
   <si>
+    <t xml:space="preserve">eth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bgd</t>
+  </si>
+  <si>
     <t xml:space="preserve">isl</t>
   </si>
   <si>
-    <t xml:space="preserve">eth</t>
-  </si>
-  <si>
     <t xml:space="preserve">uga</t>
   </si>
   <si>
-    <t xml:space="preserve">bgd</t>
-  </si>
-  <si>
     <t xml:space="preserve">phl</t>
   </si>
   <si>
+    <t xml:space="preserve">are</t>
+  </si>
+  <si>
     <t xml:space="preserve">ltu</t>
   </si>
   <si>
-    <t xml:space="preserve">are</t>
-  </si>
-  <si>
     <t xml:space="preserve">gha</t>
   </si>
   <si>
@@ -230,93 +230,96 @@
     <t xml:space="preserve">mar</t>
   </si>
   <si>
+    <t xml:space="preserve">tun</t>
+  </si>
+  <si>
     <t xml:space="preserve">ecu</t>
   </si>
   <si>
-    <t xml:space="preserve">tun</t>
-  </si>
-  <si>
     <t xml:space="preserve">lbn</t>
   </si>
   <si>
     <t xml:space="preserve">qat</t>
   </si>
   <si>
+    <t xml:space="preserve">cyp</t>
+  </si>
+  <si>
     <t xml:space="preserve">geo</t>
   </si>
   <si>
-    <t xml:space="preserve">cyp</t>
-  </si>
-  <si>
     <t xml:space="preserve">cmr</t>
   </si>
   <si>
+    <t xml:space="preserve">npl</t>
+  </si>
+  <si>
     <t xml:space="preserve">lva</t>
   </si>
   <si>
-    <t xml:space="preserve">npl</t>
-  </si>
-  <si>
     <t xml:space="preserve">lux</t>
   </si>
   <si>
+    <t xml:space="preserve">irq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mwi</t>
+  </si>
+  <si>
     <t xml:space="preserve">lka</t>
   </si>
   <si>
-    <t xml:space="preserve">mwi</t>
+    <t xml:space="preserve">ury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dza</t>
   </si>
   <si>
     <t xml:space="preserve">ven</t>
   </si>
   <si>
-    <t xml:space="preserve">ury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dza</t>
-  </si>
-  <si>
     <t xml:space="preserve">pri</t>
   </si>
   <si>
+    <t xml:space="preserve">zmb</t>
+  </si>
+  <si>
     <t xml:space="preserve">cri</t>
   </si>
   <si>
-    <t xml:space="preserve">zmb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">irq</t>
-  </si>
-  <si>
     <t xml:space="preserve">cub</t>
   </si>
   <si>
     <t xml:space="preserve">arm</t>
   </si>
   <si>
+    <t xml:space="preserve">kaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">sen</t>
   </si>
   <si>
+    <t xml:space="preserve">pan</t>
+  </si>
+  <si>
     <t xml:space="preserve">blr</t>
   </si>
   <si>
-    <t xml:space="preserve">zwe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kaz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pan</t>
+    <t xml:space="preserve">moz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdn</t>
   </si>
   <si>
     <t xml:space="preserve">bfa</t>
   </si>
   <si>
-    <t xml:space="preserve">moz</t>
-  </si>
-  <si>
     <t xml:space="preserve">mlt</t>
   </si>
   <si>
@@ -326,91 +329,91 @@
     <t xml:space="preserve">civ</t>
   </si>
   <si>
-    <t xml:space="preserve">sdn</t>
-  </si>
-  <si>
     <t xml:space="preserve">bol</t>
   </si>
   <si>
+    <t xml:space="preserve">omn</t>
+  </si>
+  <si>
     <t xml:space="preserve">cog</t>
   </si>
   <si>
-    <t xml:space="preserve">omn</t>
+    <t xml:space="preserve">mkd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rwa</t>
   </si>
   <si>
     <t xml:space="preserve">khm</t>
   </si>
   <si>
-    <t xml:space="preserve">mkd</t>
-  </si>
-  <si>
     <t xml:space="preserve">bih</t>
   </si>
   <si>
-    <t xml:space="preserve">rwa</t>
+    <t xml:space="preserve">cod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mdg</t>
   </si>
   <si>
     <t xml:space="preserve">bwa</t>
   </si>
   <si>
-    <t xml:space="preserve">mdg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cod</t>
+    <t xml:space="preserve">gtm</t>
   </si>
   <si>
     <t xml:space="preserve">ben</t>
   </si>
   <si>
-    <t xml:space="preserve">gtm</t>
+    <t xml:space="preserve">mng</t>
   </si>
   <si>
     <t xml:space="preserve">mli</t>
   </si>
   <si>
-    <t xml:space="preserve">mng</t>
-  </si>
-  <si>
     <t xml:space="preserve">mmr</t>
   </si>
   <si>
     <t xml:space="preserve">pse</t>
   </si>
   <si>
+    <t xml:space="preserve">pry</t>
+  </si>
+  <si>
     <t xml:space="preserve">alb</t>
   </si>
   <si>
+    <t xml:space="preserve">nam</t>
+  </si>
+  <si>
     <t xml:space="preserve">aze</t>
   </si>
   <si>
-    <t xml:space="preserve">pry</t>
+    <t xml:space="preserve">gmb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lao</t>
   </si>
   <si>
     <t xml:space="preserve">gab</t>
   </si>
   <si>
-    <t xml:space="preserve">gmb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nam</t>
-  </si>
-  <si>
     <t xml:space="preserve">sle</t>
   </si>
   <si>
     <t xml:space="preserve">mac</t>
   </si>
   <si>
+    <t xml:space="preserve">uzb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dom</t>
+  </si>
+  <si>
     <t xml:space="preserve">png</t>
   </si>
   <si>
-    <t xml:space="preserve">dom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uzb</t>
+    <t xml:space="preserve">lbr</t>
   </si>
   <si>
     <t xml:space="preserve">hnd</t>
@@ -419,36 +422,42 @@
     <t xml:space="preserve">mne</t>
   </si>
   <si>
+    <t xml:space="preserve">lby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bhr</t>
+  </si>
+  <si>
     <t xml:space="preserve">jam</t>
   </si>
   <si>
-    <t xml:space="preserve">gin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mda</t>
+    <t xml:space="preserve">kgz</t>
   </si>
   <si>
     <t xml:space="preserve">mco</t>
   </si>
   <si>
-    <t xml:space="preserve">lby</t>
+    <t xml:space="preserve">syr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yem</t>
   </si>
   <si>
     <t xml:space="preserve">ner</t>
   </si>
   <si>
-    <t xml:space="preserve">kgz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bhr</t>
+    <t xml:space="preserve">guf</t>
   </si>
   <si>
     <t xml:space="preserve">tgo</t>
   </si>
   <si>
-    <t xml:space="preserve">guf</t>
-  </si>
-  <si>
     <t xml:space="preserve">nic</t>
   </si>
   <si>
@@ -458,18 +467,9 @@
     <t xml:space="preserve">slv</t>
   </si>
   <si>
-    <t xml:space="preserve">syr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yem</t>
-  </si>
-  <si>
     <t xml:space="preserve">ncl</t>
   </si>
   <si>
-    <t xml:space="preserve">lbr</t>
-  </si>
-  <si>
     <t xml:space="preserve">hti</t>
   </si>
   <si>
@@ -485,33 +485,33 @@
     <t xml:space="preserve">pyf</t>
   </si>
   <si>
+    <t xml:space="preserve">swz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brn</t>
+  </si>
+  <si>
     <t xml:space="preserve">grl</t>
   </si>
   <si>
-    <t xml:space="preserve">brn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swz</t>
+    <t xml:space="preserve">afg</t>
   </si>
   <si>
     <t xml:space="preserve">caf</t>
   </si>
   <si>
-    <t xml:space="preserve">afg</t>
+    <t xml:space="preserve">ago</t>
   </si>
   <si>
     <t xml:space="preserve">syc</t>
   </si>
   <si>
+    <t xml:space="preserve">bdi</t>
+  </si>
+  <si>
     <t xml:space="preserve">glp</t>
   </si>
   <si>
-    <t xml:space="preserve">ago</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bdi</t>
-  </si>
-  <si>
     <t xml:space="preserve">btn</t>
   </si>
   <si>
@@ -521,69 +521,72 @@
     <t xml:space="preserve">gnb</t>
   </si>
   <si>
+    <t xml:space="preserve">wsm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tjk</t>
+  </si>
+  <si>
     <t xml:space="preserve">mtq</t>
   </si>
   <si>
-    <t xml:space="preserve">reu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tjk</t>
+    <t xml:space="preserve">blz</t>
   </si>
   <si>
     <t xml:space="preserve">tcd</t>
   </si>
   <si>
+    <t xml:space="preserve">sur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lso</t>
+  </si>
+  <si>
     <t xml:space="preserve">slb</t>
   </si>
   <si>
-    <t xml:space="preserve">wsm</t>
+    <t xml:space="preserve">lie</t>
   </si>
   <si>
     <t xml:space="preserve">guy</t>
   </si>
   <si>
+    <t xml:space="preserve">mrt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bhs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsm</t>
+  </si>
+  <si>
     <t xml:space="preserve">sux</t>
   </si>
   <si>
-    <t xml:space="preserve">lie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mrt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fsm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bhs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lso</t>
+    <t xml:space="preserve">cpv</t>
   </si>
   <si>
     <t xml:space="preserve">bmu</t>
   </si>
   <si>
-    <t xml:space="preserve">cpv</t>
-  </si>
-  <si>
     <t xml:space="preserve">grd</t>
   </si>
   <si>
+    <t xml:space="preserve">som</t>
+  </si>
+  <si>
     <t xml:space="preserve">and</t>
   </si>
   <si>
-    <t xml:space="preserve">som</t>
-  </si>
-  <si>
     <t xml:space="preserve">kna</t>
   </si>
   <si>
+    <t xml:space="preserve">ssd</t>
+  </si>
+  <si>
     <t xml:space="preserve">vut</t>
   </si>
   <si>
@@ -593,126 +596,123 @@
     <t xml:space="preserve">eri</t>
   </si>
   <si>
+    <t xml:space="preserve">gum</t>
+  </si>
+  <si>
     <t xml:space="preserve">smr</t>
   </si>
   <si>
-    <t xml:space="preserve">gum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssd</t>
+    <t xml:space="preserve">tls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flk</t>
   </si>
   <si>
     <t xml:space="preserve">prk</t>
   </si>
   <si>
-    <t xml:space="preserve">flk</t>
+    <t xml:space="preserve">vir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dji</t>
   </si>
   <si>
     <t xml:space="preserve">ton</t>
   </si>
   <si>
-    <t xml:space="preserve">dji</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vir</t>
+    <t xml:space="preserve">scg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cok</t>
   </si>
   <si>
     <t xml:space="preserve">ddr</t>
   </si>
   <si>
-    <t xml:space="preserve">tls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gnq</t>
+    <t xml:space="preserve">mdv</t>
   </si>
   <si>
     <t xml:space="preserve">dma</t>
   </si>
   <si>
-    <t xml:space="preserve">cok</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mdv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plw</t>
+    <t xml:space="preserve">cuw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mhl</t>
   </si>
   <si>
     <t xml:space="preserve">yug</t>
   </si>
   <si>
+    <t xml:space="preserve">asm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vgb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com</t>
+  </si>
+  <si>
     <t xml:space="preserve">vct</t>
   </si>
   <si>
-    <t xml:space="preserve">mhl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vgb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cuw</t>
-  </si>
-  <si>
     <t xml:space="preserve">ant</t>
   </si>
   <si>
-    <t xml:space="preserve">com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asm</t>
-  </si>
-  <si>
     <t xml:space="preserve">tkm</t>
   </si>
   <si>
     <t xml:space="preserve">eue</t>
   </si>
   <si>
+    <t xml:space="preserve">abw</t>
+  </si>
+  <si>
     <t xml:space="preserve">tca</t>
   </si>
   <si>
-    <t xml:space="preserve">abw</t>
+    <t xml:space="preserve">ata</t>
   </si>
   <si>
     <t xml:space="preserve">lca</t>
   </si>
   <si>
-    <t xml:space="preserve">ata</t>
+    <t xml:space="preserve">atg</t>
   </si>
   <si>
     <t xml:space="preserve">sun</t>
   </si>
   <si>
-    <t xml:space="preserve">atg</t>
+    <t xml:space="preserve">stp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vat</t>
   </si>
   <si>
     <t xml:space="preserve">mnp</t>
   </si>
   <si>
+    <t xml:space="preserve">msr</t>
+  </si>
+  <si>
     <t xml:space="preserve">sgs</t>
   </si>
   <si>
-    <t xml:space="preserve">msr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stp</t>
-  </si>
-  <si>
     <t xml:space="preserve">myt</t>
   </si>
   <si>
@@ -722,54 +722,54 @@
     <t xml:space="preserve">umi</t>
   </si>
   <si>
+    <t xml:space="preserve">niu</t>
+  </si>
+  <si>
     <t xml:space="preserve">shn</t>
   </si>
   <si>
-    <t xml:space="preserve">niu</t>
+    <t xml:space="preserve">sjm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csk</t>
   </si>
   <si>
     <t xml:space="preserve">sxm</t>
   </si>
   <si>
-    <t xml:space="preserve">csk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sjm</t>
-  </si>
-  <si>
     <t xml:space="preserve">iot</t>
   </si>
   <si>
+    <t xml:space="preserve">nru</t>
+  </si>
+  <si>
     <t xml:space="preserve">tkl</t>
   </si>
   <si>
-    <t xml:space="preserve">nru</t>
+    <t xml:space="preserve">wlf</t>
   </si>
   <si>
     <t xml:space="preserve">spm</t>
   </si>
   <si>
-    <t xml:space="preserve">wlf</t>
-  </si>
-  <si>
     <t xml:space="preserve">esh</t>
   </si>
   <si>
+    <t xml:space="preserve">rom</t>
+  </si>
+  <si>
     <t xml:space="preserve">bur</t>
   </si>
   <si>
+    <t xml:space="preserve">maf</t>
+  </si>
+  <si>
     <t xml:space="preserve">cck</t>
   </si>
   <si>
-    <t xml:space="preserve">maf</t>
-  </si>
-  <si>
     <t xml:space="preserve">bes</t>
   </si>
   <si>
-    <t xml:space="preserve">rom</t>
-  </si>
-  <si>
     <t xml:space="preserve">zar</t>
   </si>
   <si>
@@ -782,15 +782,15 @@
     <t xml:space="preserve">bvt</t>
   </si>
   <si>
+    <t xml:space="preserve">jey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cxr</t>
+  </si>
+  <si>
     <t xml:space="preserve">atf</t>
   </si>
   <si>
-    <t xml:space="preserve">cxr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jey</t>
-  </si>
-  <si>
     <t xml:space="preserve">czh</t>
   </si>
   <si>
@@ -803,10 +803,10 @@
     <t xml:space="preserve">bys</t>
   </si>
   <si>
+    <t xml:space="preserve">hvo</t>
+  </si>
+  <si>
     <t xml:space="preserve">pci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hvo</t>
   </si>
   <si>
     <t xml:space="preserve">uno</t>
@@ -1163,10 +1163,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>1402250</v>
+        <v>1523010</v>
       </c>
       <c r="C2" t="n">
-        <v>32131705</v>
+        <v>33713331</v>
       </c>
     </row>
     <row r="3">
@@ -1174,10 +1174,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>655067</v>
+        <v>709049</v>
       </c>
       <c r="C3" t="n">
-        <v>7346284</v>
+        <v>7634502</v>
       </c>
     </row>
     <row r="4">
@@ -1185,10 +1185,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>223838</v>
+        <v>242688</v>
       </c>
       <c r="C4" t="n">
-        <v>2181067</v>
+        <v>2270838</v>
       </c>
     </row>
     <row r="5">
@@ -1196,10 +1196,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>209378</v>
+        <v>226872</v>
       </c>
       <c r="C5" t="n">
-        <v>1911884</v>
+        <v>1986372</v>
       </c>
     </row>
     <row r="6">
@@ -1207,10 +1207,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>183393</v>
+        <v>195371</v>
       </c>
       <c r="C6" t="n">
-        <v>1272663</v>
+        <v>1317479</v>
       </c>
     </row>
     <row r="7">
@@ -1218,10 +1218,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>172604</v>
+        <v>186065</v>
       </c>
       <c r="C7" t="n">
-        <v>915836</v>
+        <v>960794</v>
       </c>
     </row>
     <row r="8">
@@ -1229,10 +1229,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>150496</v>
+        <v>164058</v>
       </c>
       <c r="C8" t="n">
-        <v>1774600</v>
+        <v>1842760</v>
       </c>
     </row>
     <row r="9">
@@ -1240,10 +1240,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>144688</v>
+        <v>162153</v>
       </c>
       <c r="C9" t="n">
-        <v>844085</v>
+        <v>5496033</v>
       </c>
     </row>
     <row r="10">
@@ -1251,10 +1251,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>138117</v>
+        <v>157263</v>
       </c>
       <c r="C10" t="n">
-        <v>4882015</v>
+        <v>890639</v>
       </c>
     </row>
     <row r="11">
@@ -1262,10 +1262,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>117093</v>
+        <v>127736</v>
       </c>
       <c r="C11" t="n">
-        <v>1087670</v>
+        <v>1137723</v>
       </c>
     </row>
     <row r="12">
@@ -1273,10 +1273,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>98609</v>
+        <v>108014</v>
       </c>
       <c r="C12" t="n">
-        <v>811986</v>
+        <v>855447</v>
       </c>
     </row>
     <row r="13">
@@ -1284,10 +1284,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>92173</v>
+        <v>99740</v>
       </c>
       <c r="C13" t="n">
-        <v>600040</v>
+        <v>626847</v>
       </c>
     </row>
     <row r="14">
@@ -1295,10 +1295,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>63742</v>
+        <v>69779</v>
       </c>
       <c r="C14" t="n">
-        <v>487457</v>
+        <v>510289</v>
       </c>
     </row>
     <row r="15">
@@ -1306,10 +1306,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>54422</v>
+        <v>58568</v>
       </c>
       <c r="C15" t="n">
-        <v>396079</v>
+        <v>412788</v>
       </c>
     </row>
     <row r="16">
@@ -1317,10 +1317,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>51779</v>
+        <v>57579</v>
       </c>
       <c r="C16" t="n">
-        <v>866067</v>
+        <v>915460</v>
       </c>
     </row>
     <row r="17">
@@ -1328,10 +1328,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>48339</v>
+        <v>52561</v>
       </c>
       <c r="C17" t="n">
-        <v>331692</v>
+        <v>347400</v>
       </c>
     </row>
     <row r="18">
@@ -1339,10 +1339,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>44921</v>
+        <v>50058</v>
       </c>
       <c r="C18" t="n">
-        <v>687471</v>
+        <v>736021</v>
       </c>
     </row>
     <row r="19">
@@ -1350,10 +1350,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>39208</v>
+        <v>45406</v>
       </c>
       <c r="C19" t="n">
-        <v>1278653</v>
+        <v>1382373</v>
       </c>
     </row>
     <row r="20">
@@ -1361,10 +1361,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>38234</v>
+        <v>41740</v>
       </c>
       <c r="C20" t="n">
-        <v>254181</v>
+        <v>267460</v>
       </c>
     </row>
     <row r="21">
@@ -1372,10 +1372,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>33652</v>
+        <v>36493</v>
       </c>
       <c r="C21" t="n">
-        <v>604920</v>
+        <v>633107</v>
       </c>
     </row>
     <row r="22">
@@ -1383,10 +1383,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>32208</v>
+        <v>35534</v>
       </c>
       <c r="C22" t="n">
-        <v>316541</v>
+        <v>418342</v>
       </c>
     </row>
     <row r="23">
@@ -1394,10 +1394,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>31963</v>
+        <v>34808</v>
       </c>
       <c r="C23" t="n">
-        <v>190488</v>
+        <v>332726</v>
       </c>
     </row>
     <row r="24">
@@ -1405,10 +1405,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>31756</v>
+        <v>34014</v>
       </c>
       <c r="C24" t="n">
-        <v>393451</v>
+        <v>199078</v>
       </c>
     </row>
     <row r="25">
@@ -1416,10 +1416,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>30709</v>
+        <v>33377</v>
       </c>
       <c r="C25" t="n">
-        <v>244539</v>
+        <v>256486</v>
       </c>
     </row>
     <row r="26">
@@ -1427,10 +1427,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>30316</v>
+        <v>32712</v>
       </c>
       <c r="C26" t="n">
-        <v>195958</v>
+        <v>206351</v>
       </c>
     </row>
     <row r="27">
@@ -1438,10 +1438,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>25858</v>
+        <v>28484</v>
       </c>
       <c r="C27" t="n">
-        <v>322463</v>
+        <v>344924</v>
       </c>
     </row>
     <row r="28">
@@ -1449,10 +1449,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>25142</v>
+        <v>27981</v>
       </c>
       <c r="C28" t="n">
-        <v>204294</v>
+        <v>220014</v>
       </c>
     </row>
     <row r="29">
@@ -1460,10 +1460,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>21686</v>
+        <v>23585</v>
       </c>
       <c r="C29" t="n">
-        <v>218192</v>
+        <v>227217</v>
       </c>
     </row>
     <row r="30">
@@ -1471,10 +1471,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>21139</v>
+        <v>22975</v>
       </c>
       <c r="C30" t="n">
-        <v>162749</v>
+        <v>171122</v>
       </c>
     </row>
     <row r="31">
@@ -1482,10 +1482,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>20552</v>
+        <v>22741</v>
       </c>
       <c r="C31" t="n">
-        <v>190297</v>
+        <v>201978</v>
       </c>
     </row>
     <row r="32">
@@ -1493,10 +1493,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>19935</v>
+        <v>21764</v>
       </c>
       <c r="C32" t="n">
-        <v>270928</v>
+        <v>285110</v>
       </c>
     </row>
     <row r="33">
@@ -1504,10 +1504,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>19261</v>
+        <v>21114</v>
       </c>
       <c r="C33" t="n">
-        <v>170532</v>
+        <v>178644</v>
       </c>
     </row>
     <row r="34">
@@ -1515,10 +1515,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>17491</v>
+        <v>19472</v>
       </c>
       <c r="C34" t="n">
-        <v>144537</v>
+        <v>427187</v>
       </c>
     </row>
     <row r="35">
@@ -1526,10 +1526,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="n">
-        <v>17135</v>
+        <v>19135</v>
       </c>
       <c r="C35" t="n">
-        <v>179002</v>
+        <v>193104</v>
       </c>
     </row>
     <row r="36">
@@ -1537,10 +1537,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="n">
-        <v>17095</v>
+        <v>18977</v>
       </c>
       <c r="C36" t="n">
-        <v>396980</v>
+        <v>153021</v>
       </c>
     </row>
     <row r="37">
@@ -1548,10 +1548,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="n">
-        <v>16640</v>
+        <v>18395</v>
       </c>
       <c r="C37" t="n">
-        <v>132678</v>
+        <v>141880</v>
       </c>
     </row>
     <row r="38">
@@ -1559,10 +1559,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="n">
-        <v>16293</v>
+        <v>17930</v>
       </c>
       <c r="C38" t="n">
-        <v>148290</v>
+        <v>155351</v>
       </c>
     </row>
     <row r="39">
@@ -1570,10 +1570,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>14354</v>
+        <v>16618</v>
       </c>
       <c r="C39" t="n">
-        <v>124809</v>
+        <v>180476</v>
       </c>
     </row>
     <row r="40">
@@ -1581,10 +1581,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="n">
-        <v>13389</v>
+        <v>15695</v>
       </c>
       <c r="C40" t="n">
-        <v>160155</v>
+        <v>130618</v>
       </c>
     </row>
     <row r="41">
@@ -1592,10 +1592,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="n">
-        <v>12913</v>
+        <v>14033</v>
       </c>
       <c r="C41" t="n">
-        <v>144254</v>
+        <v>150747</v>
       </c>
     </row>
     <row r="42">
@@ -1603,10 +1603,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="n">
-        <v>10220</v>
+        <v>11848</v>
       </c>
       <c r="C42" t="n">
-        <v>153047</v>
+        <v>192177</v>
       </c>
     </row>
     <row r="43">
@@ -1614,10 +1614,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="n">
-        <v>10139</v>
+        <v>11481</v>
       </c>
       <c r="C43" t="n">
-        <v>109998</v>
+        <v>163660</v>
       </c>
     </row>
     <row r="44">
@@ -1625,10 +1625,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="n">
-        <v>9988</v>
+        <v>11393</v>
       </c>
       <c r="C44" t="n">
-        <v>160041</v>
+        <v>173788</v>
       </c>
     </row>
     <row r="45">
@@ -1636,10 +1636,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="n">
-        <v>9551</v>
+        <v>11391</v>
       </c>
       <c r="C45" t="n">
-        <v>174999</v>
+        <v>116759</v>
       </c>
     </row>
     <row r="46">
@@ -1647,10 +1647,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="n">
-        <v>9164</v>
+        <v>11291</v>
       </c>
       <c r="C46" t="n">
-        <v>159429</v>
+        <v>179465</v>
       </c>
     </row>
     <row r="47">
@@ -1658,10 +1658,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="n">
-        <v>9033</v>
+        <v>10294</v>
       </c>
       <c r="C47" t="n">
-        <v>121546</v>
+        <v>132114</v>
       </c>
     </row>
     <row r="48">
@@ -1669,10 +1669,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="n">
-        <v>8498</v>
+        <v>9893</v>
       </c>
       <c r="C48" t="n">
-        <v>218826</v>
+        <v>237456</v>
       </c>
     </row>
     <row r="49">
@@ -1680,10 +1680,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="n">
-        <v>7314</v>
+        <v>8613</v>
       </c>
       <c r="C49" t="n">
-        <v>96644</v>
+        <v>105898</v>
       </c>
     </row>
     <row r="50">
@@ -1691,10 +1691,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="n">
-        <v>7080</v>
+        <v>8244</v>
       </c>
       <c r="C50" t="n">
-        <v>61060</v>
+        <v>218601</v>
       </c>
     </row>
     <row r="51">
@@ -1702,10 +1702,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="n">
-        <v>6888</v>
+        <v>7857</v>
       </c>
       <c r="C51" t="n">
-        <v>195461</v>
+        <v>64193</v>
       </c>
     </row>
     <row r="52">
@@ -1713,10 +1713,10 @@
         <v>53</v>
       </c>
       <c r="B52" t="n">
-        <v>6158</v>
+        <v>6951</v>
       </c>
       <c r="C52" t="n">
-        <v>57873</v>
+        <v>91783</v>
       </c>
     </row>
     <row r="53">
@@ -1724,10 +1724,10 @@
         <v>54</v>
       </c>
       <c r="B53" t="n">
-        <v>6095</v>
+        <v>6710</v>
       </c>
       <c r="C53" t="n">
-        <v>81108</v>
+        <v>60832</v>
       </c>
     </row>
     <row r="54">
@@ -1735,10 +1735,10 @@
         <v>55</v>
       </c>
       <c r="B54" t="n">
-        <v>5890</v>
+        <v>6422</v>
       </c>
       <c r="C54" t="n">
-        <v>48427</v>
+        <v>50916</v>
       </c>
     </row>
     <row r="55">
@@ -1746,10 +1746,10 @@
         <v>56</v>
       </c>
       <c r="B55" t="n">
-        <v>5374</v>
+        <v>5946</v>
       </c>
       <c r="C55" t="n">
-        <v>59251</v>
+        <v>41994</v>
       </c>
     </row>
     <row r="56">
@@ -1757,10 +1757,10 @@
         <v>57</v>
       </c>
       <c r="B56" t="n">
-        <v>5215</v>
+        <v>5889</v>
       </c>
       <c r="C56" t="n">
-        <v>38948</v>
+        <v>48283</v>
       </c>
     </row>
     <row r="57">
@@ -1768,10 +1768,10 @@
         <v>58</v>
       </c>
       <c r="B57" t="n">
-        <v>5090</v>
+        <v>5762</v>
       </c>
       <c r="C57" t="n">
-        <v>42080</v>
+        <v>61886</v>
       </c>
     </row>
     <row r="58">
@@ -1779,10 +1779,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="n">
-        <v>4816</v>
+        <v>5322</v>
       </c>
       <c r="C58" t="n">
-        <v>118095</v>
+        <v>125464</v>
       </c>
     </row>
     <row r="59">
@@ -1790,10 +1790,10 @@
         <v>60</v>
       </c>
       <c r="B59" t="n">
-        <v>4540</v>
+        <v>4874</v>
       </c>
       <c r="C59" t="n">
-        <v>24407</v>
+        <v>25807</v>
       </c>
     </row>
     <row r="60">
@@ -1801,10 +1801,10 @@
         <v>61</v>
       </c>
       <c r="B60" t="n">
-        <v>4453</v>
+        <v>4849</v>
       </c>
       <c r="C60" t="n">
-        <v>49802</v>
+        <v>51766</v>
       </c>
     </row>
     <row r="61">
@@ -1812,10 +1812,10 @@
         <v>62</v>
       </c>
       <c r="B61" t="n">
-        <v>4026</v>
+        <v>4516</v>
       </c>
       <c r="C61" t="n">
-        <v>17018</v>
+        <v>47089</v>
       </c>
     </row>
     <row r="62">
@@ -1823,10 +1823,10 @@
         <v>63</v>
       </c>
       <c r="B62" t="n">
-        <v>3862</v>
+        <v>4302</v>
       </c>
       <c r="C62" t="n">
-        <v>40781</v>
+        <v>68630</v>
       </c>
     </row>
     <row r="63">
@@ -1834,10 +1834,10 @@
         <v>64</v>
       </c>
       <c r="B63" t="n">
-        <v>3637</v>
+        <v>4257</v>
       </c>
       <c r="C63" t="n">
-        <v>20700</v>
+        <v>17934</v>
       </c>
     </row>
     <row r="64">
@@ -1845,10 +1845,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="n">
-        <v>3583</v>
+        <v>4194</v>
       </c>
       <c r="C64" t="n">
-        <v>61380</v>
+        <v>22712</v>
       </c>
     </row>
     <row r="65">
@@ -1856,10 +1856,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="n">
-        <v>3492</v>
+        <v>3904</v>
       </c>
       <c r="C65" t="n">
-        <v>42354</v>
+        <v>46514</v>
       </c>
     </row>
     <row r="66">
@@ -1867,10 +1867,10 @@
         <v>67</v>
       </c>
       <c r="B66" t="n">
-        <v>3297</v>
+        <v>3891</v>
       </c>
       <c r="C66" t="n">
-        <v>28927</v>
+        <v>53051</v>
       </c>
     </row>
     <row r="67">
@@ -1878,10 +1878,10 @@
         <v>68</v>
       </c>
       <c r="B67" t="n">
-        <v>3089</v>
+        <v>3613</v>
       </c>
       <c r="C67" t="n">
-        <v>46476</v>
+        <v>30635</v>
       </c>
     </row>
     <row r="68">
@@ -1889,10 +1889,10 @@
         <v>69</v>
       </c>
       <c r="B68" t="n">
-        <v>2975</v>
+        <v>3444</v>
       </c>
       <c r="C68" t="n">
-        <v>25902</v>
+        <v>29155</v>
       </c>
     </row>
     <row r="69">
@@ -1900,10 +1900,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="n">
-        <v>2759</v>
+        <v>3130</v>
       </c>
       <c r="C69" t="n">
-        <v>19566</v>
+        <v>21331</v>
       </c>
     </row>
     <row r="70">
@@ -1911,10 +1911,10 @@
         <v>71</v>
       </c>
       <c r="B70" t="n">
-        <v>2615</v>
+        <v>2962</v>
       </c>
       <c r="C70" t="n">
-        <v>52933</v>
+        <v>57624</v>
       </c>
     </row>
     <row r="71">
@@ -1922,10 +1922,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="n">
-        <v>2466</v>
+        <v>2817</v>
       </c>
       <c r="C71" t="n">
-        <v>31861</v>
+        <v>59625</v>
       </c>
     </row>
     <row r="72">
@@ -1933,10 +1933,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="n">
-        <v>2413</v>
+        <v>2787</v>
       </c>
       <c r="C72" t="n">
-        <v>56425</v>
+        <v>35886</v>
       </c>
     </row>
     <row r="73">
@@ -1944,10 +1944,10 @@
         <v>74</v>
       </c>
       <c r="B73" t="n">
-        <v>2408</v>
+        <v>2752</v>
       </c>
       <c r="C73" t="n">
-        <v>27585</v>
+        <v>29697</v>
       </c>
     </row>
     <row r="74">
@@ -1955,10 +1955,10 @@
         <v>75</v>
       </c>
       <c r="B74" t="n">
-        <v>2399</v>
+        <v>2707</v>
       </c>
       <c r="C74" t="n">
-        <v>22536</v>
+        <v>24805</v>
       </c>
     </row>
     <row r="75">
@@ -1966,10 +1966,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="n">
-        <v>2341</v>
+        <v>2640</v>
       </c>
       <c r="C75" t="n">
-        <v>20326</v>
+        <v>20066</v>
       </c>
     </row>
     <row r="76">
@@ -1977,10 +1977,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="n">
-        <v>2316</v>
+        <v>2561</v>
       </c>
       <c r="C76" t="n">
-        <v>18310</v>
+        <v>21538</v>
       </c>
     </row>
     <row r="77">
@@ -1988,10 +1988,10 @@
         <v>78</v>
       </c>
       <c r="B77" t="n">
-        <v>2104</v>
+        <v>2423</v>
       </c>
       <c r="C77" t="n">
-        <v>20029</v>
+        <v>22149</v>
       </c>
     </row>
     <row r="78">
@@ -1999,10 +1999,10 @@
         <v>79</v>
       </c>
       <c r="B78" t="n">
-        <v>2038</v>
+        <v>2335</v>
       </c>
       <c r="C78" t="n">
-        <v>16394</v>
+        <v>22410</v>
       </c>
     </row>
     <row r="79">
@@ -2010,10 +2010,10 @@
         <v>80</v>
       </c>
       <c r="B79" t="n">
-        <v>2034</v>
+        <v>2228</v>
       </c>
       <c r="C79" t="n">
-        <v>20213</v>
+        <v>17534</v>
       </c>
     </row>
     <row r="80">
@@ -2021,10 +2021,10 @@
         <v>81</v>
       </c>
       <c r="B80" t="n">
-        <v>1852</v>
+        <v>2128</v>
       </c>
       <c r="C80" t="n">
-        <v>14761</v>
+        <v>15960</v>
       </c>
     </row>
     <row r="81">
@@ -2032,10 +2032,10 @@
         <v>82</v>
       </c>
       <c r="B81" t="n">
-        <v>1743</v>
+        <v>2095</v>
       </c>
       <c r="C81" t="n">
-        <v>25026</v>
+        <v>73233</v>
       </c>
     </row>
     <row r="82">
@@ -2043,10 +2043,10 @@
         <v>83</v>
       </c>
       <c r="B82" t="n">
-        <v>1720</v>
+        <v>1960</v>
       </c>
       <c r="C82" t="n">
-        <v>8679</v>
+        <v>35764</v>
       </c>
     </row>
     <row r="83">
@@ -2054,10 +2054,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="n">
-        <v>1686</v>
+        <v>1939</v>
       </c>
       <c r="C83" t="n">
-        <v>35287</v>
+        <v>9347</v>
       </c>
     </row>
     <row r="84">
@@ -2065,10 +2065,10 @@
         <v>85</v>
       </c>
       <c r="B84" t="n">
-        <v>1676</v>
+        <v>1909</v>
       </c>
       <c r="C84" t="n">
-        <v>16629</v>
+        <v>27441</v>
       </c>
     </row>
     <row r="85">
@@ -2076,10 +2076,10 @@
         <v>86</v>
       </c>
       <c r="B85" t="n">
-        <v>1625</v>
+        <v>1892</v>
       </c>
       <c r="C85" t="n">
-        <v>32008</v>
+        <v>17653</v>
       </c>
     </row>
     <row r="86">
@@ -2087,10 +2087,10 @@
         <v>87</v>
       </c>
       <c r="B86" t="n">
-        <v>1511</v>
+        <v>1793</v>
       </c>
       <c r="C86" t="n">
-        <v>55410</v>
+        <v>59355</v>
       </c>
     </row>
     <row r="87">
@@ -2098,10 +2098,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="n">
-        <v>1502</v>
+        <v>1784</v>
       </c>
       <c r="C87" t="n">
-        <v>15695</v>
+        <v>35984</v>
       </c>
     </row>
     <row r="88">
@@ -2109,10 +2109,10 @@
         <v>89</v>
       </c>
       <c r="B88" t="n">
-        <v>1497</v>
+        <v>1696</v>
       </c>
       <c r="C88" t="n">
-        <v>13849</v>
+        <v>16661</v>
       </c>
     </row>
     <row r="89">
@@ -2120,10 +2120,10 @@
         <v>90</v>
       </c>
       <c r="B89" t="n">
-        <v>1476</v>
+        <v>1690</v>
       </c>
       <c r="C89" t="n">
-        <v>8282</v>
+        <v>9022</v>
       </c>
     </row>
     <row r="90">
@@ -2131,10 +2131,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="n">
-        <v>1460</v>
+        <v>1660</v>
       </c>
       <c r="C90" t="n">
-        <v>63626</v>
+        <v>14809</v>
       </c>
     </row>
     <row r="91">
@@ -2142,10 +2142,10 @@
         <v>92</v>
       </c>
       <c r="B91" t="n">
-        <v>1385</v>
+        <v>1509</v>
       </c>
       <c r="C91" t="n">
-        <v>38705</v>
+        <v>39885</v>
       </c>
     </row>
     <row r="92">
@@ -2153,10 +2153,10 @@
         <v>93</v>
       </c>
       <c r="B92" t="n">
-        <v>1379</v>
+        <v>1494</v>
       </c>
       <c r="C92" t="n">
-        <v>9389</v>
+        <v>9938</v>
       </c>
     </row>
     <row r="93">
@@ -2164,10 +2164,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="n">
-        <v>1239</v>
+        <v>1418</v>
       </c>
       <c r="C93" t="n">
-        <v>10350</v>
+        <v>33451</v>
       </c>
     </row>
     <row r="94">
@@ -2175,10 +2175,10 @@
         <v>95</v>
       </c>
       <c r="B94" t="n">
-        <v>1236</v>
+        <v>1408</v>
       </c>
       <c r="C94" t="n">
-        <v>20772</v>
+        <v>12238</v>
       </c>
     </row>
     <row r="95">
@@ -2186,10 +2186,10 @@
         <v>96</v>
       </c>
       <c r="B95" t="n">
-        <v>1226</v>
+        <v>1405</v>
       </c>
       <c r="C95" t="n">
-        <v>11495</v>
+        <v>11060</v>
       </c>
     </row>
     <row r="96">
@@ -2197,10 +2197,10 @@
         <v>97</v>
       </c>
       <c r="B96" t="n">
-        <v>1219</v>
+        <v>1366</v>
       </c>
       <c r="C96" t="n">
-        <v>30253</v>
+        <v>8058</v>
       </c>
     </row>
     <row r="97">
@@ -2208,10 +2208,10 @@
         <v>98</v>
       </c>
       <c r="B97" t="n">
-        <v>1213</v>
+        <v>1290</v>
       </c>
       <c r="C97" t="n">
-        <v>7336</v>
+        <v>21839</v>
       </c>
     </row>
     <row r="98">
@@ -2219,10 +2219,10 @@
         <v>99</v>
       </c>
       <c r="B98" t="n">
-        <v>1098</v>
+        <v>1226</v>
       </c>
       <c r="C98" t="n">
-        <v>7249</v>
+        <v>6057</v>
       </c>
     </row>
     <row r="99">
@@ -2230,10 +2230,10 @@
         <v>100</v>
       </c>
       <c r="B99" t="n">
-        <v>1057</v>
+        <v>1224</v>
       </c>
       <c r="C99" t="n">
-        <v>5542</v>
+        <v>15397</v>
       </c>
     </row>
     <row r="100">
@@ -2241,10 +2241,10 @@
         <v>101</v>
       </c>
       <c r="B100" t="n">
-        <v>1049</v>
+        <v>1190</v>
       </c>
       <c r="C100" t="n">
-        <v>6355</v>
+        <v>7793</v>
       </c>
     </row>
     <row r="101">
@@ -2252,10 +2252,10 @@
         <v>102</v>
       </c>
       <c r="B101" t="n">
-        <v>1027</v>
+        <v>1174</v>
       </c>
       <c r="C101" t="n">
-        <v>16904</v>
+        <v>6906</v>
       </c>
     </row>
     <row r="102">
@@ -2263,10 +2263,10 @@
         <v>103</v>
       </c>
       <c r="B102" t="n">
-        <v>1017</v>
+        <v>1171</v>
       </c>
       <c r="C102" t="n">
-        <v>8502</v>
+        <v>18028</v>
       </c>
     </row>
     <row r="103">
@@ -2274,10 +2274,10 @@
         <v>104</v>
       </c>
       <c r="B103" t="n">
-        <v>1001</v>
+        <v>1140</v>
       </c>
       <c r="C103" t="n">
-        <v>14069</v>
+        <v>9111</v>
       </c>
     </row>
     <row r="104">
@@ -2285,10 +2285,10 @@
         <v>105</v>
       </c>
       <c r="B104" t="n">
-        <v>978</v>
+        <v>1109</v>
       </c>
       <c r="C104" t="n">
-        <v>6097</v>
+        <v>6559</v>
       </c>
     </row>
     <row r="105">
@@ -2296,10 +2296,10 @@
         <v>106</v>
       </c>
       <c r="B105" t="n">
-        <v>956</v>
+        <v>1080</v>
       </c>
       <c r="C105" t="n">
-        <v>6749</v>
+        <v>17193</v>
       </c>
     </row>
     <row r="106">
@@ -2307,10 +2307,10 @@
         <v>107</v>
       </c>
       <c r="B106" t="n">
-        <v>954</v>
+        <v>1035</v>
       </c>
       <c r="C106" t="n">
-        <v>15576</v>
+        <v>7138</v>
       </c>
     </row>
     <row r="107">
@@ -2318,10 +2318,10 @@
         <v>108</v>
       </c>
       <c r="B107" t="n">
-        <v>917</v>
+        <v>1013</v>
       </c>
       <c r="C107" t="n">
-        <v>5293</v>
+        <v>9326</v>
       </c>
     </row>
     <row r="108">
@@ -2329,10 +2329,10 @@
         <v>109</v>
       </c>
       <c r="B108" t="n">
-        <v>904</v>
+        <v>1006</v>
       </c>
       <c r="C108" t="n">
-        <v>8803</v>
+        <v>6198</v>
       </c>
     </row>
     <row r="109">
@@ -2340,10 +2340,10 @@
         <v>110</v>
       </c>
       <c r="B109" t="n">
-        <v>888</v>
+        <v>1000</v>
       </c>
       <c r="C109" t="n">
-        <v>11988</v>
+        <v>5703</v>
       </c>
     </row>
     <row r="110">
@@ -2351,10 +2351,10 @@
         <v>111</v>
       </c>
       <c r="B110" t="n">
-        <v>886</v>
+        <v>978</v>
       </c>
       <c r="C110" t="n">
-        <v>5507</v>
+        <v>12881</v>
       </c>
     </row>
     <row r="111">
@@ -2362,10 +2362,10 @@
         <v>112</v>
       </c>
       <c r="B111" t="n">
-        <v>797</v>
+        <v>959</v>
       </c>
       <c r="C111" t="n">
-        <v>6191</v>
+        <v>4751</v>
       </c>
     </row>
     <row r="112">
@@ -2373,10 +2373,10 @@
         <v>113</v>
       </c>
       <c r="B112" t="n">
-        <v>793</v>
+        <v>897</v>
       </c>
       <c r="C112" t="n">
-        <v>5371</v>
+        <v>5689</v>
       </c>
     </row>
     <row r="113">
@@ -2384,10 +2384,10 @@
         <v>114</v>
       </c>
       <c r="B113" t="n">
-        <v>775</v>
+        <v>872</v>
       </c>
       <c r="C113" t="n">
-        <v>4055</v>
+        <v>6620</v>
       </c>
     </row>
     <row r="114">
@@ -2395,10 +2395,10 @@
         <v>115</v>
       </c>
       <c r="B114" t="n">
-        <v>742</v>
+        <v>840</v>
       </c>
       <c r="C114" t="n">
-        <v>6200</v>
+        <v>4661</v>
       </c>
     </row>
     <row r="115">
@@ -2406,10 +2406,10 @@
         <v>116</v>
       </c>
       <c r="B115" t="n">
-        <v>714</v>
+        <v>811</v>
       </c>
       <c r="C115" t="n">
-        <v>4314</v>
+        <v>6673</v>
       </c>
     </row>
     <row r="116">
@@ -2417,10 +2417,10 @@
         <v>117</v>
       </c>
       <c r="B116" t="n">
-        <v>708</v>
+        <v>808</v>
       </c>
       <c r="C116" t="n">
-        <v>4028</v>
+        <v>6971</v>
       </c>
     </row>
     <row r="117">
@@ -2428,10 +2428,10 @@
         <v>118</v>
       </c>
       <c r="B117" t="n">
-        <v>702</v>
+        <v>770</v>
       </c>
       <c r="C117" t="n">
-        <v>6331</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="118">
@@ -2439,10 +2439,10 @@
         <v>119</v>
       </c>
       <c r="B118" t="n">
-        <v>684</v>
+        <v>732</v>
       </c>
       <c r="C118" t="n">
-        <v>5741</v>
+        <v>6092</v>
       </c>
     </row>
     <row r="119">
@@ -2450,10 +2450,10 @@
         <v>120</v>
       </c>
       <c r="B119" t="n">
-        <v>591</v>
+        <v>671</v>
       </c>
       <c r="C119" t="n">
-        <v>7254</v>
+        <v>8124</v>
       </c>
     </row>
     <row r="120">
@@ -2461,10 +2461,10 @@
         <v>121</v>
       </c>
       <c r="B120" t="n">
-        <v>569</v>
+        <v>666</v>
       </c>
       <c r="C120" t="n">
-        <v>5348</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="121">
@@ -2472,10 +2472,10 @@
         <v>122</v>
       </c>
       <c r="B121" t="n">
-        <v>552</v>
+        <v>639</v>
       </c>
       <c r="C121" t="n">
-        <v>10348</v>
+        <v>5786</v>
       </c>
     </row>
     <row r="122">
@@ -2483,10 +2483,10 @@
         <v>123</v>
       </c>
       <c r="B122" t="n">
-        <v>550</v>
+        <v>628</v>
       </c>
       <c r="C122" t="n">
-        <v>3531</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="123">
@@ -2494,10 +2494,10 @@
         <v>124</v>
       </c>
       <c r="B123" t="n">
-        <v>543</v>
+        <v>615</v>
       </c>
       <c r="C123" t="n">
-        <v>2995</v>
+        <v>11221</v>
       </c>
     </row>
     <row r="124">
@@ -2505,10 +2505,10 @@
         <v>125</v>
       </c>
       <c r="B124" t="n">
-        <v>541</v>
+        <v>601</v>
       </c>
       <c r="C124" t="n">
-        <v>2586</v>
+        <v>2778</v>
       </c>
     </row>
     <row r="125">
@@ -2516,10 +2516,10 @@
         <v>126</v>
       </c>
       <c r="B125" t="n">
-        <v>540</v>
+        <v>589</v>
       </c>
       <c r="C125" t="n">
-        <v>3132</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="126">
@@ -2527,10 +2527,10 @@
         <v>127</v>
       </c>
       <c r="B126" t="n">
-        <v>537</v>
+        <v>587</v>
       </c>
       <c r="C126" t="n">
-        <v>3897</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="127">
@@ -2538,10 +2538,10 @@
         <v>128</v>
       </c>
       <c r="B127" t="n">
-        <v>511</v>
+        <v>587</v>
       </c>
       <c r="C127" t="n">
-        <v>2358</v>
+        <v>2587</v>
       </c>
     </row>
     <row r="128">
@@ -2549,10 +2549,10 @@
         <v>129</v>
       </c>
       <c r="B128" t="n">
-        <v>501</v>
+        <v>580</v>
       </c>
       <c r="C128" t="n">
-        <v>13297</v>
+        <v>15582</v>
       </c>
     </row>
     <row r="129">
@@ -2560,10 +2560,10 @@
         <v>130</v>
       </c>
       <c r="B129" t="n">
-        <v>493</v>
+        <v>553</v>
       </c>
       <c r="C129" t="n">
-        <v>4089</v>
+        <v>16129</v>
       </c>
     </row>
     <row r="130">
@@ -2571,10 +2571,10 @@
         <v>131</v>
       </c>
       <c r="B130" t="n">
-        <v>468</v>
+        <v>544</v>
       </c>
       <c r="C130" t="n">
-        <v>2902</v>
+        <v>3064</v>
       </c>
     </row>
     <row r="131">
@@ -2582,10 +2582,10 @@
         <v>132</v>
       </c>
       <c r="B131" t="n">
-        <v>460</v>
+        <v>544</v>
       </c>
       <c r="C131" t="n">
-        <v>14029</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="132">
@@ -2593,10 +2593,10 @@
         <v>133</v>
       </c>
       <c r="B132" t="n">
-        <v>453</v>
+        <v>519</v>
       </c>
       <c r="C132" t="n">
-        <v>2500</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="133">
@@ -2604,10 +2604,10 @@
         <v>134</v>
       </c>
       <c r="B133" t="n">
-        <v>414</v>
+        <v>507</v>
       </c>
       <c r="C133" t="n">
-        <v>2916</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="134">
@@ -2615,10 +2615,10 @@
         <v>135</v>
       </c>
       <c r="B134" t="n">
-        <v>398</v>
+        <v>453</v>
       </c>
       <c r="C134" t="n">
-        <v>6799</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="135">
@@ -2626,10 +2626,10 @@
         <v>136</v>
       </c>
       <c r="B135" t="n">
-        <v>389</v>
+        <v>449</v>
       </c>
       <c r="C135" t="n">
-        <v>1833</v>
+        <v>8075</v>
       </c>
     </row>
     <row r="136">
@@ -2637,10 +2637,10 @@
         <v>137</v>
       </c>
       <c r="B136" t="n">
-        <v>380</v>
+        <v>438</v>
       </c>
       <c r="C136" t="n">
-        <v>4971</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="137">
@@ -2648,10 +2648,10 @@
         <v>138</v>
       </c>
       <c r="B137" t="n">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C137" t="n">
-        <v>1858</v>
+        <v>5251</v>
       </c>
     </row>
     <row r="138">
@@ -2659,10 +2659,10 @@
         <v>139</v>
       </c>
       <c r="B138" t="n">
-        <v>363</v>
+        <v>419</v>
       </c>
       <c r="C138" t="n">
-        <v>7506</v>
+        <v>7337</v>
       </c>
     </row>
     <row r="139">
@@ -2670,10 +2670,10 @@
         <v>140</v>
       </c>
       <c r="B139" t="n">
-        <v>362</v>
+        <v>419</v>
       </c>
       <c r="C139" t="n">
-        <v>2915</v>
+        <v>7020</v>
       </c>
     </row>
     <row r="140">
@@ -2681,10 +2681,10 @@
         <v>141</v>
       </c>
       <c r="B140" t="n">
-        <v>350</v>
+        <v>399</v>
       </c>
       <c r="C140" t="n">
-        <v>3353</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="141">
@@ -2692,10 +2692,10 @@
         <v>142</v>
       </c>
       <c r="B141" t="n">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c r="C141" t="n">
-        <v>6585</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="142">
@@ -2703,10 +2703,10 @@
         <v>143</v>
       </c>
       <c r="B142" t="n">
-        <v>336</v>
+        <v>392</v>
       </c>
       <c r="C142" t="n">
-        <v>2476</v>
+        <v>8330</v>
       </c>
     </row>
     <row r="143">
@@ -2714,10 +2714,10 @@
         <v>144</v>
       </c>
       <c r="B143" t="n">
-        <v>326</v>
+        <v>388</v>
       </c>
       <c r="C143" t="n">
-        <v>1702</v>
+        <v>6675</v>
       </c>
     </row>
     <row r="144">
@@ -2725,10 +2725,10 @@
         <v>145</v>
       </c>
       <c r="B144" t="n">
-        <v>317</v>
+        <v>385</v>
       </c>
       <c r="C144" t="n">
-        <v>2158</v>
+        <v>3108</v>
       </c>
     </row>
     <row r="145">
@@ -2736,10 +2736,10 @@
         <v>146</v>
       </c>
       <c r="B145" t="n">
-        <v>305</v>
+        <v>367</v>
       </c>
       <c r="C145" t="n">
-        <v>3513</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="146">
@@ -2747,10 +2747,10 @@
         <v>147</v>
       </c>
       <c r="B146" t="n">
-        <v>299</v>
+        <v>359</v>
       </c>
       <c r="C146" t="n">
-        <v>2244</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="147">
@@ -2758,10 +2758,10 @@
         <v>148</v>
       </c>
       <c r="B147" t="n">
-        <v>289</v>
+        <v>334</v>
       </c>
       <c r="C147" t="n">
-        <v>7497</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="148">
@@ -2769,10 +2769,10 @@
         <v>149</v>
       </c>
       <c r="B148" t="n">
-        <v>289</v>
+        <v>332</v>
       </c>
       <c r="C148" t="n">
-        <v>5881</v>
+        <v>3734</v>
       </c>
     </row>
     <row r="149">
@@ -2780,10 +2780,10 @@
         <v>150</v>
       </c>
       <c r="B149" t="n">
-        <v>273</v>
+        <v>327</v>
       </c>
       <c r="C149" t="n">
-        <v>2410</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="150">
@@ -2791,10 +2791,10 @@
         <v>151</v>
       </c>
       <c r="B150" t="n">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="C150" t="n">
-        <v>1407</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="151">
@@ -2802,10 +2802,10 @@
         <v>152</v>
       </c>
       <c r="B151" t="n">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="C151" t="n">
-        <v>1694</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="152">
@@ -2813,10 +2813,10 @@
         <v>153</v>
       </c>
       <c r="B152" t="n">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="C152" t="n">
-        <v>5654</v>
+        <v>5889</v>
       </c>
     </row>
     <row r="153">
@@ -2824,10 +2824,10 @@
         <v>154</v>
       </c>
       <c r="B153" t="n">
-        <v>241</v>
+        <v>272</v>
       </c>
       <c r="C153" t="n">
-        <v>2954</v>
+        <v>3164</v>
       </c>
     </row>
     <row r="154">
@@ -2835,10 +2835,10 @@
         <v>155</v>
       </c>
       <c r="B154" t="n">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="C154" t="n">
-        <v>1760</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="155">
@@ -2846,10 +2846,10 @@
         <v>156</v>
       </c>
       <c r="B155" t="n">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="C155" t="n">
-        <v>1634</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="156">
@@ -2857,10 +2857,10 @@
         <v>157</v>
       </c>
       <c r="B156" t="n">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C156" t="n">
-        <v>1205</v>
+        <v>2303</v>
       </c>
     </row>
     <row r="157">
@@ -2868,10 +2868,10 @@
         <v>158</v>
       </c>
       <c r="B157" t="n">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="C157" t="n">
-        <v>4033</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="158">
@@ -2879,10 +2879,10 @@
         <v>159</v>
       </c>
       <c r="B158" t="n">
-        <v>193</v>
+        <v>222</v>
       </c>
       <c r="C158" t="n">
-        <v>2195</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="159">
@@ -2890,10 +2890,10 @@
         <v>160</v>
       </c>
       <c r="B159" t="n">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="C159" t="n">
-        <v>1131</v>
+        <v>3592</v>
       </c>
     </row>
     <row r="160">
@@ -2901,10 +2901,10 @@
         <v>161</v>
       </c>
       <c r="B160" t="n">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="C160" t="n">
-        <v>3217</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="161">
@@ -2912,10 +2912,10 @@
         <v>162</v>
       </c>
       <c r="B161" t="n">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C161" t="n">
-        <v>787</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="162">
@@ -2923,10 +2923,10 @@
         <v>163</v>
       </c>
       <c r="B162" t="n">
-        <v>138</v>
+        <v>167</v>
       </c>
       <c r="C162" t="n">
-        <v>1627</v>
+        <v>824</v>
       </c>
     </row>
     <row r="163">
@@ -2934,10 +2934,10 @@
         <v>164</v>
       </c>
       <c r="B163" t="n">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C163" t="n">
-        <v>1711</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="164">
@@ -2945,10 +2945,10 @@
         <v>165</v>
       </c>
       <c r="B164" t="n">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="C164" t="n">
-        <v>1017</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="165">
@@ -2956,10 +2956,10 @@
         <v>166</v>
       </c>
       <c r="B165" t="n">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C165" t="n">
-        <v>1429</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="166">
@@ -2967,10 +2967,10 @@
         <v>167</v>
       </c>
       <c r="B166" t="n">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C166" t="n">
-        <v>807</v>
+        <v>862</v>
       </c>
     </row>
     <row r="167">
@@ -2978,10 +2978,10 @@
         <v>168</v>
       </c>
       <c r="B167" t="n">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C167" t="n">
-        <v>611</v>
+        <v>639</v>
       </c>
     </row>
     <row r="168">
@@ -2989,10 +2989,10 @@
         <v>169</v>
       </c>
       <c r="B168" t="n">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C168" t="n">
-        <v>986</v>
+        <v>688</v>
       </c>
     </row>
     <row r="169">
@@ -3000,10 +3000,10 @@
         <v>170</v>
       </c>
       <c r="B169" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="C169" t="n">
-        <v>1181</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="170">
@@ -3011,10 +3011,10 @@
         <v>171</v>
       </c>
       <c r="B170" t="n">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C170" t="n">
-        <v>1914</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="171">
@@ -3022,10 +3022,10 @@
         <v>172</v>
       </c>
       <c r="B171" t="n">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C171" t="n">
-        <v>844</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="172">
@@ -3033,10 +3033,10 @@
         <v>173</v>
       </c>
       <c r="B172" t="n">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C172" t="n">
-        <v>776</v>
+        <v>765</v>
       </c>
     </row>
     <row r="173">
@@ -3044,10 +3044,10 @@
         <v>174</v>
       </c>
       <c r="B173" t="n">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="C173" t="n">
-        <v>630</v>
+        <v>930</v>
       </c>
     </row>
     <row r="174">
@@ -3055,10 +3055,10 @@
         <v>175</v>
       </c>
       <c r="B174" t="n">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C174" t="n">
-        <v>1066</v>
+        <v>820</v>
       </c>
     </row>
     <row r="175">
@@ -3066,10 +3066,10 @@
         <v>176</v>
       </c>
       <c r="B175" t="n">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C175" t="n">
-        <v>37035</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="176">
@@ -3077,10 +3077,10 @@
         <v>177</v>
       </c>
       <c r="B176" t="n">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C176" t="n">
-        <v>1325</v>
+        <v>791</v>
       </c>
     </row>
     <row r="177">
@@ -3088,10 +3088,10 @@
         <v>178</v>
       </c>
       <c r="B177" t="n">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C177" t="n">
-        <v>719</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="178">
@@ -3099,10 +3099,10 @@
         <v>179</v>
       </c>
       <c r="B178" t="n">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C178" t="n">
-        <v>768</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="179">
@@ -3110,10 +3110,10 @@
         <v>180</v>
       </c>
       <c r="B179" t="n">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C179" t="n">
-        <v>970</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="180">
@@ -3121,10 +3121,10 @@
         <v>181</v>
       </c>
       <c r="B180" t="n">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C180" t="n">
-        <v>330</v>
+        <v>793</v>
       </c>
     </row>
     <row r="181">
@@ -3132,10 +3132,10 @@
         <v>182</v>
       </c>
       <c r="B181" t="n">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C181" t="n">
-        <v>741</v>
+        <v>341</v>
       </c>
     </row>
     <row r="182">
@@ -3143,10 +3143,10 @@
         <v>183</v>
       </c>
       <c r="B182" t="n">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C182" t="n">
-        <v>1098</v>
+        <v>37032</v>
       </c>
     </row>
     <row r="183">
@@ -3154,10 +3154,10 @@
         <v>184</v>
       </c>
       <c r="B183" t="n">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C183" t="n">
-        <v>803</v>
+        <v>645</v>
       </c>
     </row>
     <row r="184">
@@ -3165,10 +3165,10 @@
         <v>185</v>
       </c>
       <c r="B184" t="n">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C184" t="n">
-        <v>582</v>
+        <v>820</v>
       </c>
     </row>
     <row r="185">
@@ -3176,10 +3176,10 @@
         <v>186</v>
       </c>
       <c r="B185" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C185" t="n">
-        <v>1954</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="186">
@@ -3187,10 +3187,10 @@
         <v>187</v>
       </c>
       <c r="B186" t="n">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C186" t="n">
-        <v>336</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="187">
@@ -3198,10 +3198,10 @@
         <v>188</v>
       </c>
       <c r="B187" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C187" t="n">
-        <v>906</v>
+        <v>368</v>
       </c>
     </row>
     <row r="188">
@@ -3209,10 +3209,10 @@
         <v>189</v>
       </c>
       <c r="B188" t="n">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C188" t="n">
-        <v>806</v>
+        <v>874</v>
       </c>
     </row>
     <row r="189">
@@ -3220,10 +3220,10 @@
         <v>190</v>
       </c>
       <c r="B189" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C189" t="n">
-        <v>550</v>
+        <v>407</v>
       </c>
     </row>
     <row r="190">
@@ -3231,10 +3231,10 @@
         <v>191</v>
       </c>
       <c r="B190" t="n">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C190" t="n">
-        <v>153</v>
+        <v>570</v>
       </c>
     </row>
     <row r="191">
@@ -3242,10 +3242,10 @@
         <v>192</v>
       </c>
       <c r="B191" t="n">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C191" t="n">
-        <v>863</v>
+        <v>161</v>
       </c>
     </row>
     <row r="192">
@@ -3253,10 +3253,10 @@
         <v>193</v>
       </c>
       <c r="B192" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C192" t="n">
-        <v>325</v>
+        <v>944</v>
       </c>
     </row>
     <row r="193">
@@ -3264,10 +3264,10 @@
         <v>194</v>
       </c>
       <c r="B193" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C193" t="n">
-        <v>836</v>
+        <v>885</v>
       </c>
     </row>
     <row r="194">
@@ -3275,10 +3275,10 @@
         <v>195</v>
       </c>
       <c r="B194" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C194" t="n">
-        <v>335</v>
+        <v>350</v>
       </c>
     </row>
     <row r="195">
@@ -3286,10 +3286,10 @@
         <v>196</v>
       </c>
       <c r="B195" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C195" t="n">
-        <v>1591</v>
+        <v>482</v>
       </c>
     </row>
     <row r="196">
@@ -3297,10 +3297,10 @@
         <v>197</v>
       </c>
       <c r="B196" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C196" t="n">
-        <v>303</v>
+        <v>314</v>
       </c>
     </row>
     <row r="197">
@@ -3308,10 +3308,10 @@
         <v>198</v>
       </c>
       <c r="B197" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C197" t="n">
-        <v>277</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="198">
@@ -3319,10 +3319,10 @@
         <v>199</v>
       </c>
       <c r="B198" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C198" t="n">
-        <v>407</v>
+        <v>329</v>
       </c>
     </row>
     <row r="199">
@@ -3330,10 +3330,10 @@
         <v>200</v>
       </c>
       <c r="B199" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C199" t="n">
-        <v>299</v>
+        <v>335</v>
       </c>
     </row>
     <row r="200">
@@ -3341,10 +3341,10 @@
         <v>201</v>
       </c>
       <c r="B200" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C200" t="n">
-        <v>11720</v>
+        <v>434</v>
       </c>
     </row>
     <row r="201">
@@ -3352,10 +3352,10 @@
         <v>202</v>
       </c>
       <c r="B201" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C201" t="n">
-        <v>426</v>
+        <v>288</v>
       </c>
     </row>
     <row r="202">
@@ -3363,10 +3363,10 @@
         <v>203</v>
       </c>
       <c r="B202" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C202" t="n">
-        <v>9733</v>
+        <v>9748</v>
       </c>
     </row>
     <row r="203">
@@ -3374,10 +3374,10 @@
         <v>204</v>
       </c>
       <c r="B203" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C203" t="n">
-        <v>316</v>
+        <v>260</v>
       </c>
     </row>
     <row r="204">
@@ -3385,10 +3385,10 @@
         <v>205</v>
       </c>
       <c r="B204" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C204" t="n">
-        <v>413</v>
+        <v>143</v>
       </c>
     </row>
     <row r="205">
@@ -3396,10 +3396,10 @@
         <v>206</v>
       </c>
       <c r="B205" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C205" t="n">
-        <v>133</v>
+        <v>11738</v>
       </c>
     </row>
     <row r="206">
@@ -3407,10 +3407,10 @@
         <v>207</v>
       </c>
       <c r="B206" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C206" t="n">
-        <v>490</v>
+        <v>564</v>
       </c>
     </row>
     <row r="207">
@@ -3418,10 +3418,10 @@
         <v>208</v>
       </c>
       <c r="B207" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C207" t="n">
-        <v>246</v>
+        <v>435</v>
       </c>
     </row>
     <row r="208">
@@ -3429,10 +3429,10 @@
         <v>209</v>
       </c>
       <c r="B208" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C208" t="n">
-        <v>8077</v>
+        <v>157</v>
       </c>
     </row>
     <row r="209">
@@ -3440,10 +3440,10 @@
         <v>210</v>
       </c>
       <c r="B209" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C209" t="n">
-        <v>511</v>
+        <v>258</v>
       </c>
     </row>
     <row r="210">
@@ -3451,10 +3451,10 @@
         <v>211</v>
       </c>
       <c r="B210" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C210" t="n">
-        <v>162</v>
+        <v>358</v>
       </c>
     </row>
     <row r="211">
@@ -3462,10 +3462,10 @@
         <v>212</v>
       </c>
       <c r="B211" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C211" t="n">
-        <v>339</v>
+        <v>169</v>
       </c>
     </row>
     <row r="212">
@@ -3473,10 +3473,10 @@
         <v>213</v>
       </c>
       <c r="B212" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C212" t="n">
-        <v>218</v>
+        <v>8105</v>
       </c>
     </row>
     <row r="213">
@@ -3484,10 +3484,10 @@
         <v>214</v>
       </c>
       <c r="B213" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C213" t="n">
-        <v>164</v>
+        <v>274</v>
       </c>
     </row>
     <row r="214">
@@ -3495,10 +3495,10 @@
         <v>215</v>
       </c>
       <c r="B214" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C214" t="n">
-        <v>2694</v>
+        <v>2698</v>
       </c>
     </row>
     <row r="215">
@@ -3506,10 +3506,10 @@
         <v>216</v>
       </c>
       <c r="B215" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C215" t="n">
-        <v>121</v>
+        <v>167</v>
       </c>
     </row>
     <row r="216">
@@ -3517,10 +3517,10 @@
         <v>217</v>
       </c>
       <c r="B216" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C216" t="n">
-        <v>448</v>
+        <v>277</v>
       </c>
     </row>
     <row r="217">
@@ -3528,10 +3528,10 @@
         <v>218</v>
       </c>
       <c r="B217" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C217" t="n">
-        <v>261</v>
+        <v>512</v>
       </c>
     </row>
     <row r="218">
@@ -3539,10 +3539,10 @@
         <v>219</v>
       </c>
       <c r="B218" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C218" t="n">
-        <v>262</v>
+        <v>454</v>
       </c>
     </row>
     <row r="219">
@@ -3550,10 +3550,10 @@
         <v>220</v>
       </c>
       <c r="B219" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C219" t="n">
-        <v>328</v>
+        <v>365</v>
       </c>
     </row>
     <row r="220">
@@ -3561,10 +3561,10 @@
         <v>221</v>
       </c>
       <c r="B220" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C220" t="n">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="221">
@@ -3572,10 +3572,10 @@
         <v>222</v>
       </c>
       <c r="B221" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C221" t="n">
-        <v>101</v>
+        <v>225</v>
       </c>
     </row>
     <row r="222">
@@ -3583,10 +3583,10 @@
         <v>223</v>
       </c>
       <c r="B222" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C222" t="n">
-        <v>207</v>
+        <v>106</v>
       </c>
     </row>
     <row r="223">
@@ -3594,10 +3594,10 @@
         <v>224</v>
       </c>
       <c r="B223" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C223" t="n">
-        <v>250</v>
+        <v>79</v>
       </c>
     </row>
     <row r="224">
@@ -3605,10 +3605,10 @@
         <v>225</v>
       </c>
       <c r="B224" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C224" t="n">
-        <v>74</v>
+        <v>256</v>
       </c>
     </row>
     <row r="225">
@@ -3616,10 +3616,10 @@
         <v>226</v>
       </c>
       <c r="B225" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C225" t="n">
-        <v>1281</v>
+        <v>326</v>
       </c>
     </row>
     <row r="226">
@@ -3627,10 +3627,10 @@
         <v>227</v>
       </c>
       <c r="B226" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C226" t="n">
-        <v>294</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="227">
@@ -3638,10 +3638,10 @@
         <v>228</v>
       </c>
       <c r="B227" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C227" t="n">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="228">
@@ -3649,10 +3649,10 @@
         <v>229</v>
       </c>
       <c r="B228" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C228" t="n">
-        <v>60</v>
+        <v>104</v>
       </c>
     </row>
     <row r="229">
@@ -3660,10 +3660,10 @@
         <v>230</v>
       </c>
       <c r="B229" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C229" t="n">
-        <v>122</v>
+        <v>146</v>
       </c>
     </row>
     <row r="230">
@@ -3671,10 +3671,10 @@
         <v>231</v>
       </c>
       <c r="B230" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C230" t="n">
-        <v>92</v>
+        <v>129</v>
       </c>
     </row>
     <row r="231">
@@ -3682,10 +3682,10 @@
         <v>232</v>
       </c>
       <c r="B231" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C231" t="n">
-        <v>139</v>
+        <v>62</v>
       </c>
     </row>
     <row r="232">
@@ -3693,10 +3693,10 @@
         <v>233</v>
       </c>
       <c r="B232" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C232" t="n">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="233">
@@ -3704,10 +3704,10 @@
         <v>234</v>
       </c>
       <c r="B233" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C233" t="n">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="234">
@@ -3729,7 +3729,7 @@
         <v>6</v>
       </c>
       <c r="C235" t="n">
-        <v>82</v>
+        <v>29</v>
       </c>
     </row>
     <row r="236">
@@ -3737,10 +3737,10 @@
         <v>237</v>
       </c>
       <c r="B236" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C236" t="n">
-        <v>28</v>
+        <v>83</v>
       </c>
     </row>
     <row r="237">
@@ -3748,10 +3748,10 @@
         <v>238</v>
       </c>
       <c r="B237" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C237" t="n">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="238">
@@ -3762,7 +3762,7 @@
         <v>5</v>
       </c>
       <c r="C238" t="n">
-        <v>1063</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="239">
@@ -3773,7 +3773,7 @@
         <v>5</v>
       </c>
       <c r="C239" t="n">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="240">
@@ -3784,7 +3784,7 @@
         <v>5</v>
       </c>
       <c r="C240" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="241">
@@ -3792,10 +3792,10 @@
         <v>242</v>
       </c>
       <c r="B241" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C241" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="242">
@@ -3803,10 +3803,10 @@
         <v>243</v>
       </c>
       <c r="B242" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C242" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="243">
@@ -3817,7 +3817,7 @@
         <v>3</v>
       </c>
       <c r="C243" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="244">
@@ -3825,10 +3825,10 @@
         <v>245</v>
       </c>
       <c r="B244" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C244" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
     </row>
     <row r="245">
@@ -3850,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="C246" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="247">
@@ -3861,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="C247" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="248">
@@ -3872,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="C248" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="249">
@@ -3883,7 +3883,7 @@
         <v>1</v>
       </c>
       <c r="C249" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="250">
@@ -3894,7 +3894,7 @@
         <v>1</v>
       </c>
       <c r="C250" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="251">
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="C251" t="n">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="252">
@@ -3949,7 +3949,7 @@
         <v>0</v>
       </c>
       <c r="C255" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256">
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="C257" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="258">

</xml_diff>